<commit_message>
add table-generator and controllers
</commit_message>
<xml_diff>
--- a/wdc_libs/xlsx-converter/template.xlsx
+++ b/wdc_libs/xlsx-converter/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="5" r:id="rId1"/>
@@ -80,12 +80,6 @@
     <t>dataset.note</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>ua</t>
-  </si>
-  <si>
     <t>dataset.label</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>Імя стовпчика, який містить значення</t>
+  </si>
+  <si>
+    <t>value.en</t>
+  </si>
+  <si>
+    <t>value.ua</t>
   </si>
 </sst>
 </file>
@@ -148,7 +148,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -245,7 +245,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -551,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -632,10 +632,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,76 +733,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>